<commit_message>
chore: argparse instead of static input file paths
</commit_message>
<xml_diff>
--- a/BA_tasks.xlsx
+++ b/BA_tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212457E1-7BF5-D643-8371-A9F5C4248F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D850DD17-5F98-2442-9D2F-29E263B133E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5080" yWindow="1900" windowWidth="28240" windowHeight="17240" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
+    <workbookView xWindow="39520" yWindow="760" windowWidth="32920" windowHeight="17240" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -572,14 +572,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD62869-7C5A-4D40-80FD-07ED57F6AF52}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.83203125" style="3"/>
-    <col min="2" max="2" width="41.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="45.5" style="2" customWidth="1"/>
     <col min="4" max="4" width="62.5" style="10" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
fix: commented tfidf: max dense vector< vocab size
</commit_message>
<xml_diff>
--- a/BA_tasks.xlsx
+++ b/BA_tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{355C6B33-96C9-4444-97F1-9B76DDB8CAEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFC3C99-5A9F-E647-A697-A741FE16D96C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
+    <workbookView xWindow="38420" yWindow="840" windowWidth="34560" windowHeight="19400" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Task</t>
   </si>
@@ -114,6 +114,12 @@
   </si>
   <si>
     <t>pdf2image auf Cluster, visualized 9 most similar images for sample query as matrix</t>
+  </si>
+  <si>
+    <t>tfidf: document term matrix, cosine similarity, tfidf vectorization of ocument corpus</t>
+  </si>
+  <si>
+    <t>PROBLEM: Elasticsearch max. dimension of dense vector is 2048, vocab size of corpus is bigger (7243)</t>
   </si>
 </sst>
 </file>
@@ -319,8 +325,8 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -643,8 +649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD62869-7C5A-4D40-80FD-07ED57F6AF52}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -762,7 +768,7 @@
       <c r="A11" s="13">
         <v>45149</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="14" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="8" t="s">
@@ -778,6 +784,17 @@
       </c>
       <c r="D12" s="8" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="18">
+        <v>45151</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
feat: added google's universal-sentence-encoder
</commit_message>
<xml_diff>
--- a/BA_tasks.xlsx
+++ b/BA_tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFC3C99-5A9F-E647-A697-A741FE16D96C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8A2DB2-7C57-CA4D-8AE6-2FBCDDE7BBF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38420" yWindow="840" windowWidth="34560" windowHeight="19400" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Task</t>
   </si>
@@ -116,10 +116,13 @@
     <t>pdf2image auf Cluster, visualized 9 most similar images for sample query as matrix</t>
   </si>
   <si>
-    <t>tfidf: document term matrix, cosine similarity, tfidf vectorization of ocument corpus</t>
-  </si>
-  <si>
     <t>PROBLEM: Elasticsearch max. dimension of dense vector is 2048, vocab size of corpus is bigger (7243)</t>
+  </si>
+  <si>
+    <t>save trained models</t>
+  </si>
+  <si>
+    <t>tfidf: document term matrix, cosine similarity, tfidf vectorization of ocument corpus, google's universal-sentence-encoder</t>
   </si>
 </sst>
 </file>
@@ -647,10 +650,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD62869-7C5A-4D40-80FD-07ED57F6AF52}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:C14"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -786,15 +789,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="18">
         <v>45151</v>
       </c>
       <c r="B13" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -805,6 +808,11 @@
     <row r="17" spans="4:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D17" s="8" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D18" s="8" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
style: deleted obsolete imports
</commit_message>
<xml_diff>
--- a/BA_tasks.xlsx
+++ b/BA_tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8A2DB2-7C57-CA4D-8AE6-2FBCDDE7BBF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04646C29-FFA2-3649-A09B-F7DA11981950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38420" yWindow="840" windowWidth="34560" windowHeight="19400" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Task</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>tfidf: document term matrix, cosine similarity, tfidf vectorization of ocument corpus, google's universal-sentence-encoder</t>
+  </si>
+  <si>
+    <t>nferSent – Supervised Learning of Sentence Embeddings/Attention mechanism etc.: https://yashuseth.wordpress.com/2018/08/06/infersent-supervised-learning-of-sentence-embeddings/</t>
   </si>
 </sst>
 </file>
@@ -650,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD62869-7C5A-4D40-80FD-07ED57F6AF52}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -815,6 +818,11 @@
         <v>27</v>
       </c>
     </row>
+    <row r="19" spans="4:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="D19" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:A5"/>

</xml_diff>

<commit_message>
feat: init, load, save huggingface sentenceTransf.
</commit_message>
<xml_diff>
--- a/BA_tasks.xlsx
+++ b/BA_tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04646C29-FFA2-3649-A09B-F7DA11981950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AFB7F4D-B916-164D-9275-30F4AED38FDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38420" yWindow="840" windowWidth="34560" windowHeight="19400" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
+    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="19400" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Task</t>
   </si>
@@ -125,7 +125,13 @@
     <t>tfidf: document term matrix, cosine similarity, tfidf vectorization of ocument corpus, google's universal-sentence-encoder</t>
   </si>
   <si>
-    <t>nferSent – Supervised Learning of Sentence Embeddings/Attention mechanism etc.: https://yashuseth.wordpress.com/2018/08/06/infersent-supervised-learning-of-sentence-embeddings/</t>
+    <t>InferSent – Supervised Learning of Sentence Embeddings/Attention mechanism etc.: https://yashuseth.wordpress.com/2018/08/06/infersent-supervised-learning-of-sentence-embeddings/</t>
+  </si>
+  <si>
+    <t>infer pretrained sentence encoder without db, bc embedding is too big for maximum dense vector size</t>
+  </si>
+  <si>
+    <t>huggingface: init, save, load sentence transformer</t>
   </si>
 </sst>
 </file>
@@ -656,7 +662,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -803,7 +809,21 @@
         <v>26</v>
       </c>
     </row>
+    <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="18">
+        <v>45152</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="18">
+        <v>45153</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>31</v>
+      </c>
       <c r="D15" s="8" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
feat:added huggingface sentence transformer column
</commit_message>
<xml_diff>
--- a/BA_tasks.xlsx
+++ b/BA_tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AFB7F4D-B916-164D-9275-30F4AED38FDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5FC140-A5AA-A046-B508-2A34543684A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="19400" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
@@ -131,7 +131,7 @@
     <t>infer pretrained sentence encoder without db, bc embedding is too big for maximum dense vector size</t>
   </si>
   <si>
-    <t>huggingface: init, save, load sentence transformer</t>
+    <t>huggingface: init, save, load sentence transformer, added as embedding to elasticSearch db</t>
   </si>
 </sst>
 </file>
@@ -328,6 +328,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -335,9 +338,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -662,7 +662,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -686,7 +686,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="15">
+      <c r="A2" s="16">
         <v>45144</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -697,7 +697,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="16"/>
+      <c r="A3" s="17"/>
       <c r="B3" s="9" t="s">
         <v>5</v>
       </c>
@@ -706,7 +706,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="16"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
@@ -715,7 +715,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="10" t="s">
         <v>8</v>
       </c>
@@ -798,30 +798,30 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A13" s="18">
+    <row r="13" spans="1:4" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
         <v>45151</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="18">
+    <row r="14" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13">
         <v>45152</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="18">
+    <row r="15" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15">
         <v>45153</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="10" t="s">
         <v>31</v>
       </c>
       <c r="D15" s="8" t="s">

</xml_diff>

<commit_message>
style: InferSent training not possible (source)
</commit_message>
<xml_diff>
--- a/BA_tasks.xlsx
+++ b/BA_tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50F25BC-254A-074E-BADD-4E459E4FD1F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021E9276-D878-4C43-8B86-66988A437B01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Task</t>
   </si>
@@ -101,9 +101,6 @@
     <t>tfidf: document term matrix, cosine similarity, tfidf vectorization of ocument corpus, google's universal-sentence-encoder</t>
   </si>
   <si>
-    <t>InferSent – Supervised Learning of Sentence Embeddings/Attention mechanism etc.: https://yashuseth.wordpress.com/2018/08/06/infersent-supervised-learning-of-sentence-embeddings/</t>
-  </si>
-  <si>
     <t>infer pretrained sentence encoder without db, bc embedding is too big for maximum dense vector size</t>
   </si>
   <si>
@@ -122,12 +119,6 @@
     <t>Usage Sentence embeddings rather than word embeddings? Ann. Beschreiben</t>
   </si>
   <si>
-    <t>multiple tfidf vectors for different tasks (1. similarity between documents omitting words which occur only once in the corpus, 2. finding specific documents omitting words which occur in every document, etc.) -&gt; reduce vector size (=#unique words)</t>
-  </si>
-  <si>
-    <t>InferSent: is there '.train' to retrain on own corpus with little effort?</t>
-  </si>
-  <si>
     <t>Google's universal Sentence Encoder: Alter shapes to fix problem</t>
   </si>
   <si>
@@ -140,10 +131,13 @@
     <t>analysis/ evaluation ideas cf. Notability 23.08.2023</t>
   </si>
   <si>
-    <t>BA: assumption is that there are similarities (content wise and in terms of visual appearance) between documents of same type (eg. Urkunde)</t>
-  </si>
-  <si>
     <t xml:space="preserve">read Universal Encoder paper, log path != result path (sbatch skripts on cluster), </t>
+  </si>
+  <si>
+    <t>InferSent: project does not support training: https://github.com/facebookresearch/InferSent/issues/82</t>
+  </si>
+  <si>
+    <t>multiple tfidf vectors for different tasks (1. similarity between documents omitting words which occur only once in the corpus, 2. finding specific documents omitting words which occur in every document, etc.) -&gt; reduce vector size (=#unique words), BA: assumption is that there are similarities (content wise and in terms of visual appearance) between documents of same type (eg. Urkunde)</t>
   </si>
 </sst>
 </file>
@@ -373,7 +367,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -695,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD62869-7C5A-4D40-80FD-07ED57F6AF52}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B19" sqref="A19:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -788,7 +782,7 @@
         <v>45148</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>11</v>
@@ -832,10 +826,10 @@
         <v>45152</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
@@ -843,71 +837,65 @@
         <v>45153</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22">
         <v>45161</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>35</v>
+      <c r="B17" s="14" t="s">
+        <v>31</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="137" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="13">
+        <v>45162</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>33</v>
+      </c>
       <c r="D18" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="D19" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="D21" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="D22" s="8" t="s">
-        <v>29</v>
+    <row r="19" spans="1:4" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="13">
+        <v>45163</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D23" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="D24" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="D25" s="8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D26" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="D27" s="8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: first work on eigenfaces
</commit_message>
<xml_diff>
--- a/BA_tasks.xlsx
+++ b/BA_tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021E9276-D878-4C43-8B86-66988A437B01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C5C82C-2339-8942-B713-D32360D85BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>Task</t>
   </si>
@@ -119,9 +119,6 @@
     <t>Usage Sentence embeddings rather than word embeddings? Ann. Beschreiben</t>
   </si>
   <si>
-    <t>Google's universal Sentence Encoder: Alter shapes to fix problem</t>
-  </si>
-  <si>
     <t>Compare .png of documents using either 1. AE, 2. Eigenface/-phase (cf. PCA), 3. from paper</t>
   </si>
   <si>
@@ -134,10 +131,16 @@
     <t xml:space="preserve">read Universal Encoder paper, log path != result path (sbatch skripts on cluster), </t>
   </si>
   <si>
-    <t>InferSent: project does not support training: https://github.com/facebookresearch/InferSent/issues/82</t>
-  </si>
-  <si>
     <t>multiple tfidf vectors for different tasks (1. similarity between documents omitting words which occur only once in the corpus, 2. finding specific documents omitting words which occur in every document, etc.) -&gt; reduce vector size (=#unique words), BA: assumption is that there are similarities (content wise and in terms of visual appearance) between documents of same type (eg. Urkunde)</t>
+  </si>
+  <si>
+    <t>Google's universal Sentence Encoder: Alter shapes to fix problem (HOW?)</t>
+  </si>
+  <si>
+    <t>make TFIDF searchable</t>
+  </si>
+  <si>
+    <t>InferSent hypothese: project does not support training: https://github.com/facebookresearch/InferSent/issues/82 , Universal Sentence Encoder: the embedding uses n-grams of documents close to current doc (like a window) to embed it, cf. DAN in https://amitness.com/2020/06/universal-sentence-encoder/ -&gt; unable to fix subtraction problem, started working on eigenfaces</t>
   </si>
 </sst>
 </file>
@@ -691,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD62869-7C5A-4D40-80FD-07ED57F6AF52}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B19" sqref="A19:B19"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -853,7 +856,7 @@
         <v>45161</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>15</v>
@@ -864,38 +867,43 @@
         <v>45162</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="154" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13">
         <v>45163</v>
       </c>
       <c r="B19" s="14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D22" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="D23" s="8" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="D23" s="8" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="D24" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="D25" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D26" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: PCA transform to 2 dim
</commit_message>
<xml_diff>
--- a/BA_tasks.xlsx
+++ b/BA_tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C5C82C-2339-8942-B713-D32360D85BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3817270-4C4B-3141-A0C0-8DE406FF1601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
+    <workbookView xWindow="38400" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>Task</t>
   </si>
@@ -141,6 +141,12 @@
   </si>
   <si>
     <t>InferSent hypothese: project does not support training: https://github.com/facebookresearch/InferSent/issues/82 , Universal Sentence Encoder: the embedding uses n-grams of documents close to current doc (like a window) to embed it, cf. DAN in https://amitness.com/2020/06/universal-sentence-encoder/ -&gt; unable to fix subtraction problem, started working on eigenfaces</t>
+  </si>
+  <si>
+    <t>cluster PCA results of images</t>
+  </si>
+  <si>
+    <t>why are cluster sizes of PCA results imbalanced?</t>
   </si>
 </sst>
 </file>
@@ -692,10 +698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD62869-7C5A-4D40-80FD-07ED57F6AF52}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B20" sqref="A20:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -881,6 +887,14 @@
         <v>34</v>
       </c>
     </row>
+    <row r="20" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="13">
+        <v>45164</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>35</v>
+      </c>
+    </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D22" s="8" t="s">
         <v>33</v>
@@ -904,6 +918,11 @@
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D26" s="8" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D27" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: added strip accents to tfidf emb in db
</commit_message>
<xml_diff>
--- a/BA_tasks.xlsx
+++ b/BA_tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB660058-049F-A24C-8DEB-BAD8AB2C2E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8426CF7F-EA3F-BA41-8BAD-D14DBCD777E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="1580" windowWidth="34560" windowHeight="19880" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
+    <workbookView xWindow="38400" yWindow="1520" windowWidth="34560" windowHeight="19880" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -146,9 +146,6 @@
     <t xml:space="preserve">PROBLEM: Elasticsearch max. dimension of dense vector is 2048, vocab size of corpus is bigger (7243), SOLUTION: create multple features/ properties for large vector and search multiple times when querying OR use PCA/ AE to reduce dimensionality </t>
   </si>
   <si>
-    <t>TFIDF: strip accents</t>
-  </si>
-  <si>
     <t>TFIDF: automatic preprocessing? Ggf. stemming/ lemmatization (using NLTK) to reduce vocabulary</t>
   </si>
   <si>
@@ -216,6 +213,9 @@
   </si>
   <si>
     <t>Lizenzen: GPL kann man nicht so einfach nutzen</t>
+  </si>
+  <si>
+    <t>TFIDF: strip accents in db embedding</t>
   </si>
 </sst>
 </file>
@@ -427,6 +427,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -436,16 +442,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -769,8 +769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD62869-7C5A-4D40-80FD-07ED57F6AF52}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -794,7 +794,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="16">
+      <c r="A2" s="18">
         <v>45144</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -805,7 +805,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="17"/>
+      <c r="A3" s="19"/>
       <c r="B3" s="9" t="s">
         <v>5</v>
       </c>
@@ -814,7 +814,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="17"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
@@ -823,7 +823,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
+      <c r="A5" s="20"/>
       <c r="B5" s="10" t="s">
         <v>8</v>
       </c>
@@ -866,7 +866,7 @@
       <c r="A9" s="13">
         <v>45147</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="14" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="8" t="s">
@@ -877,7 +877,7 @@
       <c r="A10" s="13">
         <v>45148</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="14" t="s">
         <v>20</v>
       </c>
       <c r="D10" s="8" t="s">
@@ -924,9 +924,6 @@
       <c r="B14" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="8" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="15" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
@@ -936,40 +933,40 @@
         <v>19</v>
       </c>
       <c r="D15" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
     <row r="17" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="22">
+      <c r="A17" s="21">
         <v>45161</v>
       </c>
       <c r="B17" s="14" t="s">
         <v>27</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="137" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
         <v>45162</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="14" t="s">
         <v>28</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="154" thickBot="1" x14ac:dyDescent="0.25">
@@ -980,7 +977,7 @@
         <v>30</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -991,7 +988,7 @@
         <v>31</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="86" thickBot="1" x14ac:dyDescent="0.25">
@@ -1002,7 +999,7 @@
         <v>33</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -1013,82 +1010,88 @@
         <v>34</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="22">
+        <v>45168</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="D23" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="D24" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D25" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D26" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D27" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="D28" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="D29" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D30" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="D31" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D32" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="4:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D33" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="4:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D34" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="4:4" ht="51" x14ac:dyDescent="0.2">
       <c r="D35" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="4:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D36" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="4:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D37" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: added tfidf preprocessing steps
</commit_message>
<xml_diff>
--- a/BA_tasks.xlsx
+++ b/BA_tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8426CF7F-EA3F-BA41-8BAD-D14DBCD777E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50467BDF-B16B-FF40-A9B2-BAE560BEFE90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="1520" windowWidth="34560" windowHeight="19880" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
@@ -134,9 +134,6 @@
     <t>cluster PCA results of images</t>
   </si>
   <si>
-    <t>why are cluster sizes of PCA results imbalanced?</t>
-  </si>
-  <si>
     <t>solved errors of PCA clustering, added PCA-Cluster to database, DB has to be deleted to update index (!!!), deleted one tfidf embedding since it is too big, other tfidf is null vector (Problem!), db is searchable for same cluster documents</t>
   </si>
   <si>
@@ -216,6 +213,9 @@
   </si>
   <si>
     <t>TFIDF: strip accents in db embedding</t>
+  </si>
+  <si>
+    <t>why are cluster sizes of PCA results imbalanced? Because they are too sparse</t>
   </si>
 </sst>
 </file>
@@ -769,8 +769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD62869-7C5A-4D40-80FD-07ED57F6AF52}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -839,7 +839,7 @@
         <v>7</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
@@ -914,7 +914,7 @@
         <v>17</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
@@ -933,7 +933,7 @@
         <v>19</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
@@ -944,7 +944,7 @@
         <v>22</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
@@ -955,7 +955,7 @@
         <v>27</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="137" thickBot="1" x14ac:dyDescent="0.25">
@@ -966,7 +966,7 @@
         <v>28</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="154" thickBot="1" x14ac:dyDescent="0.25">
@@ -977,7 +977,7 @@
         <v>30</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -988,7 +988,7 @@
         <v>31</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="86" thickBot="1" x14ac:dyDescent="0.25">
@@ -996,10 +996,10 @@
         <v>45167</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -1007,10 +1007,10 @@
         <v>45168</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1018,80 +1018,80 @@
         <v>45168</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="D24" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D25" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D26" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D27" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="D28" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="D29" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D30" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="D31" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D32" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="4:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D33" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="4:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D34" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="4:4" ht="51" x14ac:dyDescent="0.2">
       <c r="D35" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="4:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D36" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37" spans="4:4" ht="17" x14ac:dyDescent="0.2">
       <c r="D37" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: custom preprocessor usable in TfidfVectorizer
</commit_message>
<xml_diff>
--- a/BA_tasks.xlsx
+++ b/BA_tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klara/Developer/Uni/topic-analysis-text-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50467BDF-B16B-FF40-A9B2-BAE560BEFE90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A332DA12-135F-7748-BD63-23B400104CEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="1520" windowWidth="34560" windowHeight="19880" xr2:uid="{F95BA5CE-2858-5E49-83EB-51CF4F2E8B01}"/>
   </bookViews>
@@ -212,10 +212,10 @@
     <t>Lizenzen: GPL kann man nicht so einfach nutzen</t>
   </si>
   <si>
-    <t>TFIDF: strip accents in db embedding</t>
-  </si>
-  <si>
     <t>why are cluster sizes of PCA results imbalanced? Because they are too sparse</t>
+  </si>
+  <si>
+    <t>TFIDF: strip accents in db embedding, created preprocessing class which can be used instead of default preprocessor</t>
   </si>
 </sst>
 </file>
@@ -769,8 +769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD62869-7C5A-4D40-80FD-07ED57F6AF52}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -914,7 +914,7 @@
         <v>17</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
@@ -1013,12 +1013,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="22">
         <v>45168</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>43</v>

</xml_diff>